<commit_message>
update week1 for the spring of 2025
</commit_message>
<xml_diff>
--- a/week04/array-illustration.xlsx
+++ b/week04/array-illustration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yushiqi/git/CPP/week04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836400FE-1871-654E-B4C8-8ABB91EE9C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EABF0E-D89F-FA49-99D2-A5EA99A29B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="500" windowWidth="50040" windowHeight="28300" xr2:uid="{65DC6EA1-CAD2-DA43-82E3-93A6944CF004}"/>
+    <workbookView xWindow="1220" yWindow="500" windowWidth="36580" windowHeight="28300" xr2:uid="{65DC6EA1-CAD2-DA43-82E3-93A6944CF004}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1430,6 +1430,15 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1442,30 +1451,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1477,15 +1486,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3110,9 +3110,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3150,7 +3150,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3256,7 +3256,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3398,7 +3398,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3408,8 +3408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E610120C-2380-2A44-9250-E87FF4DB0425}">
   <dimension ref="A3:CH219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="50" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="U97" sqref="U96:U97"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="50" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="L80" sqref="L80:L83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3709,19 +3709,19 @@
       </c>
     </row>
     <row r="9" spans="12:86" ht="20">
-      <c r="Q9" s="102">
+      <c r="Q9" s="104">
         <v>3</v>
       </c>
-      <c r="R9" s="100">
+      <c r="R9" s="102">
         <v>6</v>
       </c>
       <c r="S9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="V9" s="102" t="s">
+      <c r="V9" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="W9" s="100">
+      <c r="W9" s="102">
         <v>16</v>
       </c>
       <c r="X9" s="7" t="s">
@@ -3790,13 +3790,13 @@
       </c>
     </row>
     <row r="10" spans="12:86" ht="20">
-      <c r="Q10" s="102"/>
-      <c r="R10" s="100"/>
+      <c r="Q10" s="104"/>
+      <c r="R10" s="102"/>
       <c r="S10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="V10" s="102"/>
-      <c r="W10" s="100"/>
+      <c r="V10" s="104"/>
+      <c r="W10" s="102"/>
       <c r="X10" s="7" t="s">
         <v>16</v>
       </c>
@@ -3862,13 +3862,13 @@
       <c r="M11" t="s">
         <v>111</v>
       </c>
-      <c r="Q11" s="102"/>
-      <c r="R11" s="100"/>
+      <c r="Q11" s="104"/>
+      <c r="R11" s="102"/>
       <c r="S11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="V11" s="102"/>
-      <c r="W11" s="100"/>
+      <c r="V11" s="104"/>
+      <c r="W11" s="102"/>
       <c r="X11" s="7" t="s">
         <v>17</v>
       </c>
@@ -3928,13 +3928,13 @@
       <c r="M12" t="s">
         <v>108</v>
       </c>
-      <c r="Q12" s="102"/>
-      <c r="R12" s="100"/>
+      <c r="Q12" s="104"/>
+      <c r="R12" s="102"/>
       <c r="S12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="V12" s="102"/>
-      <c r="W12" s="100"/>
+      <c r="V12" s="104"/>
+      <c r="W12" s="102"/>
       <c r="X12" s="7" t="s">
         <v>18</v>
       </c>
@@ -3968,7 +3968,7 @@
       <c r="BK12" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="BL12" s="95">
+      <c r="BL12" s="98">
         <v>2002</v>
       </c>
       <c r="BM12" t="s">
@@ -3996,19 +3996,19 @@
       <c r="M13" t="s">
         <v>107</v>
       </c>
-      <c r="Q13" s="102">
+      <c r="Q13" s="104">
         <v>2</v>
       </c>
-      <c r="R13" s="100">
+      <c r="R13" s="102">
         <v>7</v>
       </c>
       <c r="S13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="V13" s="102" t="s">
+      <c r="V13" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="W13" s="100">
+      <c r="W13" s="102">
         <v>15</v>
       </c>
       <c r="X13" s="7" t="s">
@@ -4021,14 +4021,14 @@
       <c r="AD13" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="AE13" s="103"/>
+      <c r="AE13" s="105"/>
       <c r="AF13">
         <v>11</v>
       </c>
       <c r="AH13" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="AI13" s="103"/>
+      <c r="AI13" s="105"/>
       <c r="AJ13">
         <v>11</v>
       </c>
@@ -4048,7 +4048,7 @@
       <c r="BG13" s="28"/>
       <c r="BH13" s="24"/>
       <c r="BK13" s="66"/>
-      <c r="BL13" s="95"/>
+      <c r="BL13" s="98"/>
       <c r="BM13" t="s">
         <v>123</v>
       </c>
@@ -4084,13 +4084,13 @@
       <c r="M14" t="s">
         <v>106</v>
       </c>
-      <c r="Q14" s="102"/>
-      <c r="R14" s="100"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="102"/>
       <c r="S14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="V14" s="102"/>
-      <c r="W14" s="100"/>
+      <c r="V14" s="104"/>
+      <c r="W14" s="102"/>
       <c r="X14" s="7" t="s">
         <v>20</v>
       </c>
@@ -4099,12 +4099,12 @@
         <v>9</v>
       </c>
       <c r="AD14" s="66"/>
-      <c r="AE14" s="103"/>
+      <c r="AE14" s="105"/>
       <c r="AF14">
         <v>10</v>
       </c>
       <c r="AH14" s="66"/>
-      <c r="AI14" s="103"/>
+      <c r="AI14" s="105"/>
       <c r="AJ14">
         <v>10</v>
       </c>
@@ -4136,7 +4136,7 @@
       <c r="BG14" s="29"/>
       <c r="BH14" s="24"/>
       <c r="BK14" s="66"/>
-      <c r="BL14" s="95"/>
+      <c r="BL14" s="98"/>
       <c r="BM14" t="s">
         <v>124</v>
       </c>
@@ -4171,13 +4171,13 @@
       <c r="M15" t="s">
         <v>105</v>
       </c>
-      <c r="Q15" s="102"/>
-      <c r="R15" s="100"/>
+      <c r="Q15" s="104"/>
+      <c r="R15" s="102"/>
       <c r="S15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="V15" s="102"/>
-      <c r="W15" s="100"/>
+      <c r="V15" s="104"/>
+      <c r="W15" s="102"/>
       <c r="X15" s="7" t="s">
         <v>21</v>
       </c>
@@ -4191,12 +4191,12 @@
         <v>8</v>
       </c>
       <c r="AD15" s="66"/>
-      <c r="AE15" s="103"/>
+      <c r="AE15" s="105"/>
       <c r="AF15">
         <v>9</v>
       </c>
       <c r="AH15" s="66"/>
-      <c r="AI15" s="103"/>
+      <c r="AI15" s="105"/>
       <c r="AJ15">
         <v>9</v>
       </c>
@@ -4236,7 +4236,7 @@
       </c>
       <c r="BH15" s="24"/>
       <c r="BK15" s="66"/>
-      <c r="BL15" s="95"/>
+      <c r="BL15" s="98"/>
       <c r="BM15" t="s">
         <v>125</v>
       </c>
@@ -4267,32 +4267,32 @@
       <c r="M16" t="s">
         <v>110</v>
       </c>
-      <c r="Q16" s="102"/>
-      <c r="R16" s="100"/>
+      <c r="Q16" s="104"/>
+      <c r="R16" s="102"/>
       <c r="S16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="V16" s="102"/>
-      <c r="W16" s="100"/>
+      <c r="V16" s="104"/>
+      <c r="W16" s="102"/>
       <c r="X16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="Z16" s="102" t="s">
+      <c r="Z16" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="AA16" s="95">
+      <c r="AA16" s="98">
         <v>2000</v>
       </c>
       <c r="AB16">
         <v>7</v>
       </c>
       <c r="AD16" s="66"/>
-      <c r="AE16" s="103"/>
+      <c r="AE16" s="105"/>
       <c r="AF16">
         <v>8</v>
       </c>
       <c r="AH16" s="66"/>
-      <c r="AI16" s="103"/>
+      <c r="AI16" s="105"/>
       <c r="AJ16">
         <v>8</v>
       </c>
@@ -4353,26 +4353,26 @@
       <c r="M17" t="s">
         <v>109</v>
       </c>
-      <c r="Q17" s="102">
+      <c r="Q17" s="104">
         <v>1</v>
       </c>
-      <c r="R17" s="100">
+      <c r="R17" s="102">
         <v>8</v>
       </c>
       <c r="S17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="V17" s="102" t="s">
+      <c r="V17" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="W17" s="100">
+      <c r="W17" s="102">
         <v>14</v>
       </c>
       <c r="X17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Z17" s="102"/>
-      <c r="AA17" s="95"/>
+      <c r="Z17" s="104"/>
+      <c r="AA17" s="98"/>
       <c r="AB17">
         <v>6</v>
       </c>
@@ -4437,18 +4437,18 @@
       </c>
     </row>
     <row r="18" spans="12:86" ht="20">
-      <c r="Q18" s="102"/>
-      <c r="R18" s="100"/>
+      <c r="Q18" s="104"/>
+      <c r="R18" s="102"/>
       <c r="S18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="V18" s="102"/>
-      <c r="W18" s="100"/>
+      <c r="V18" s="104"/>
+      <c r="W18" s="102"/>
       <c r="X18" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Z18" s="102"/>
-      <c r="AA18" s="95"/>
+      <c r="Z18" s="104"/>
+      <c r="AA18" s="98"/>
       <c r="AB18">
         <v>5</v>
       </c>
@@ -4509,18 +4509,18 @@
       </c>
     </row>
     <row r="19" spans="12:86" ht="20">
-      <c r="Q19" s="102"/>
-      <c r="R19" s="100"/>
+      <c r="Q19" s="104"/>
+      <c r="R19" s="102"/>
       <c r="S19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="V19" s="102"/>
-      <c r="W19" s="100"/>
+      <c r="V19" s="104"/>
+      <c r="W19" s="102"/>
       <c r="X19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="Z19" s="102"/>
-      <c r="AA19" s="95"/>
+      <c r="Z19" s="104"/>
+      <c r="AA19" s="98"/>
       <c r="AB19">
         <v>4</v>
       </c>
@@ -4597,17 +4597,17 @@
       </c>
     </row>
     <row r="20" spans="12:86" ht="20">
-      <c r="Q20" s="102"/>
-      <c r="R20" s="100"/>
+      <c r="Q20" s="104"/>
+      <c r="R20" s="102"/>
       <c r="S20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="V20" s="102"/>
-      <c r="W20" s="100"/>
+      <c r="V20" s="104"/>
+      <c r="W20" s="102"/>
       <c r="X20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z20" s="102" t="s">
+      <c r="Z20" s="104" t="s">
         <v>50</v>
       </c>
       <c r="AA20" s="15">
@@ -4673,25 +4673,25 @@
       </c>
     </row>
     <row r="21" spans="12:86" ht="20">
-      <c r="Q21" s="102">
+      <c r="Q21" s="104">
         <v>0</v>
       </c>
-      <c r="R21" s="100">
+      <c r="R21" s="102">
         <v>9</v>
       </c>
       <c r="S21" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="V21" s="102" t="s">
+      <c r="V21" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="W21" s="100">
+      <c r="W21" s="102">
         <v>13</v>
       </c>
       <c r="X21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Z21" s="102"/>
+      <c r="Z21" s="104"/>
       <c r="AA21" s="15">
         <v>0</v>
       </c>
@@ -4701,21 +4701,21 @@
       <c r="AD21" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="AE21" s="103"/>
+      <c r="AE21" s="105"/>
       <c r="AF21">
         <v>3</v>
       </c>
       <c r="AH21" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="AI21" s="103"/>
+      <c r="AI21" s="105"/>
       <c r="AJ21">
         <v>3</v>
       </c>
       <c r="AL21" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="AM21" s="104" t="s">
+      <c r="AM21" s="107" t="s">
         <v>62</v>
       </c>
       <c r="AN21" s="39">
@@ -4772,17 +4772,17 @@
       </c>
     </row>
     <row r="22" spans="12:86" ht="20">
-      <c r="Q22" s="102"/>
-      <c r="R22" s="100"/>
+      <c r="Q22" s="104"/>
+      <c r="R22" s="102"/>
       <c r="S22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="V22" s="102"/>
-      <c r="W22" s="100"/>
+      <c r="V22" s="104"/>
+      <c r="W22" s="102"/>
       <c r="X22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Z22" s="102"/>
+      <c r="Z22" s="104"/>
       <c r="AA22" s="16" t="s">
         <v>54</v>
       </c>
@@ -4790,19 +4790,19 @@
         <v>1</v>
       </c>
       <c r="AD22" s="66"/>
-      <c r="AE22" s="103"/>
+      <c r="AE22" s="105"/>
       <c r="AF22">
         <v>2</v>
       </c>
       <c r="AH22" s="66"/>
-      <c r="AI22" s="103"/>
+      <c r="AI22" s="105"/>
       <c r="AJ22">
         <v>2</v>
       </c>
       <c r="AL22" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="AM22" s="105"/>
+      <c r="AM22" s="108"/>
       <c r="AN22" s="39">
         <v>0</v>
       </c>
@@ -4847,17 +4847,17 @@
       </c>
     </row>
     <row r="23" spans="12:86" ht="20">
-      <c r="Q23" s="102"/>
-      <c r="R23" s="100"/>
+      <c r="Q23" s="104"/>
+      <c r="R23" s="102"/>
       <c r="S23" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="V23" s="102"/>
-      <c r="W23" s="100"/>
+      <c r="V23" s="104"/>
+      <c r="W23" s="102"/>
       <c r="X23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="Z23" s="102"/>
+      <c r="Z23" s="104"/>
       <c r="AA23" s="16" t="s">
         <v>53</v>
       </c>
@@ -4865,19 +4865,19 @@
         <v>0</v>
       </c>
       <c r="AD23" s="66"/>
-      <c r="AE23" s="103"/>
+      <c r="AE23" s="105"/>
       <c r="AF23">
         <v>1</v>
       </c>
       <c r="AH23" s="66"/>
-      <c r="AI23" s="103"/>
+      <c r="AI23" s="105"/>
       <c r="AJ23">
         <v>1</v>
       </c>
       <c r="AL23" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="AM23" s="105"/>
+      <c r="AM23" s="108"/>
       <c r="AN23" s="39">
         <v>0</v>
       </c>
@@ -4902,7 +4902,7 @@
       <c r="BK23" s="90" t="s">
         <v>129</v>
       </c>
-      <c r="BL23" s="107" t="s">
+      <c r="BL23" s="110" t="s">
         <v>69</v>
       </c>
       <c r="BP23" s="82"/>
@@ -4926,13 +4926,13 @@
       </c>
     </row>
     <row r="24" spans="12:86" ht="20">
-      <c r="Q24" s="102"/>
-      <c r="R24" s="100"/>
+      <c r="Q24" s="104"/>
+      <c r="R24" s="102"/>
       <c r="S24" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="V24" s="102"/>
-      <c r="W24" s="100"/>
+      <c r="V24" s="104"/>
+      <c r="W24" s="102"/>
       <c r="X24" s="7" t="s">
         <v>10</v>
       </c>
@@ -4941,19 +4941,19 @@
         <v>-1</v>
       </c>
       <c r="AD24" s="66"/>
-      <c r="AE24" s="103"/>
+      <c r="AE24" s="105"/>
       <c r="AF24">
         <v>0</v>
       </c>
       <c r="AH24" s="66"/>
-      <c r="AI24" s="103"/>
+      <c r="AI24" s="105"/>
       <c r="AJ24">
         <v>0</v>
       </c>
       <c r="AL24" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="AM24" s="106"/>
+      <c r="AM24" s="109"/>
       <c r="AN24" s="39">
         <v>1</v>
       </c>
@@ -4962,7 +4962,7 @@
       </c>
       <c r="AQ24" s="1"/>
       <c r="BK24" s="90"/>
-      <c r="BL24" s="107"/>
+      <c r="BL24" s="110"/>
       <c r="BP24" s="82"/>
       <c r="BQ24" s="84"/>
       <c r="BR24" t="s">
@@ -4988,10 +4988,10 @@
       <c r="S25" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="V25" s="102" t="s">
+      <c r="V25" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="W25" s="100">
+      <c r="W25" s="102">
         <v>12</v>
       </c>
       <c r="X25" s="7" t="s">
@@ -5010,7 +5010,7 @@
         <v>63</v>
       </c>
       <c r="BK25" s="90"/>
-      <c r="BL25" s="107"/>
+      <c r="BL25" s="110"/>
       <c r="BP25" s="44"/>
       <c r="BQ25" s="45"/>
       <c r="BX25" s="51"/>
@@ -5027,8 +5027,8 @@
       <c r="S26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="V26" s="102"/>
-      <c r="W26" s="100"/>
+      <c r="V26" s="104"/>
+      <c r="W26" s="102"/>
       <c r="X26" s="7" t="s">
         <v>12</v>
       </c>
@@ -5040,7 +5040,7 @@
       <c r="AN26" s="23"/>
       <c r="AO26" s="22"/>
       <c r="BK26" s="90"/>
-      <c r="BL26" s="107"/>
+      <c r="BL26" s="110"/>
       <c r="BX26" s="51"/>
       <c r="BY26" s="51"/>
       <c r="CA26" s="5"/>
@@ -5055,8 +5055,8 @@
       <c r="S27" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="V27" s="102"/>
-      <c r="W27" s="100"/>
+      <c r="V27" s="104"/>
+      <c r="W27" s="102"/>
       <c r="X27" s="7" t="s">
         <v>13</v>
       </c>
@@ -5067,8 +5067,8 @@
       <c r="S28" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="V28" s="102"/>
-      <c r="W28" s="100"/>
+      <c r="V28" s="104"/>
+      <c r="W28" s="102"/>
       <c r="X28" s="7" t="s">
         <v>14</v>
       </c>
@@ -5076,10 +5076,10 @@
     <row r="29" spans="12:86" ht="20">
       <c r="R29" s="5"/>
       <c r="S29" s="6"/>
-      <c r="V29" s="102" t="s">
+      <c r="V29" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="W29" s="100">
+      <c r="W29" s="102">
         <v>11</v>
       </c>
       <c r="X29" s="7" t="s">
@@ -5088,24 +5088,24 @@
     </row>
     <row r="30" spans="12:86" ht="20">
       <c r="S30" s="6"/>
-      <c r="V30" s="102"/>
-      <c r="W30" s="100"/>
+      <c r="V30" s="104"/>
+      <c r="W30" s="102"/>
       <c r="X30" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="12:86" ht="20">
       <c r="S31" s="6"/>
-      <c r="V31" s="102"/>
-      <c r="W31" s="100"/>
+      <c r="V31" s="104"/>
+      <c r="W31" s="102"/>
       <c r="X31" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="12:86" ht="20">
       <c r="S32" s="6"/>
-      <c r="V32" s="102"/>
-      <c r="W32" s="101"/>
+      <c r="V32" s="104"/>
+      <c r="W32" s="103"/>
       <c r="X32" s="7" t="s">
         <v>0</v>
       </c>
@@ -5139,8 +5139,8 @@
       <c r="H39" s="50"/>
       <c r="I39" s="50"/>
       <c r="J39" s="50"/>
-      <c r="K39" s="96"/>
-      <c r="L39" s="99"/>
+      <c r="K39" s="92"/>
+      <c r="L39" s="106"/>
       <c r="M39" s="51"/>
       <c r="N39" s="51"/>
       <c r="O39" s="51"/>
@@ -5150,7 +5150,7 @@
       <c r="H40" s="50"/>
       <c r="I40" s="50"/>
       <c r="J40" s="50"/>
-      <c r="K40" s="96"/>
+      <c r="K40" s="92"/>
       <c r="L40" s="87"/>
       <c r="M40" s="51"/>
       <c r="N40" s="51"/>
@@ -5164,7 +5164,7 @@
       <c r="H41" s="50"/>
       <c r="I41" s="50"/>
       <c r="J41" s="50"/>
-      <c r="K41" s="96"/>
+      <c r="K41" s="92"/>
       <c r="L41" s="87"/>
       <c r="M41" s="51"/>
       <c r="N41" s="51"/>
@@ -5180,7 +5180,7 @@
       <c r="H42" s="50"/>
       <c r="I42" s="50"/>
       <c r="J42" s="50"/>
-      <c r="K42" s="96"/>
+      <c r="K42" s="92"/>
       <c r="L42" s="87"/>
       <c r="M42" s="51"/>
       <c r="N42" s="51"/>
@@ -5196,9 +5196,9 @@
       <c r="H43" s="50"/>
       <c r="I43" s="50"/>
       <c r="J43" s="50"/>
-      <c r="K43" s="96"/>
+      <c r="K43" s="92"/>
       <c r="L43" s="87"/>
-      <c r="M43" s="97" t="s">
+      <c r="M43" s="93" t="s">
         <v>76</v>
       </c>
       <c r="N43" s="51"/>
@@ -5214,9 +5214,9 @@
       <c r="H44" s="50"/>
       <c r="I44" s="50"/>
       <c r="J44" s="50"/>
-      <c r="K44" s="96"/>
+      <c r="K44" s="92"/>
       <c r="L44" s="87"/>
-      <c r="M44" s="97"/>
+      <c r="M44" s="93"/>
       <c r="N44" s="51"/>
       <c r="O44" s="51"/>
       <c r="P44" s="51"/>
@@ -5230,7 +5230,7 @@
       <c r="H45" s="50"/>
       <c r="I45" s="50"/>
       <c r="J45" s="50"/>
-      <c r="K45" s="96" t="s">
+      <c r="K45" s="92" t="s">
         <v>78</v>
       </c>
       <c r="L45" s="87"/>
@@ -5248,7 +5248,7 @@
       <c r="H46" s="50"/>
       <c r="I46" s="50"/>
       <c r="J46" s="50"/>
-      <c r="K46" s="96"/>
+      <c r="K46" s="92"/>
       <c r="L46" s="87"/>
       <c r="M46" s="51"/>
       <c r="N46" s="51"/>
@@ -5264,7 +5264,7 @@
       <c r="H47" s="50"/>
       <c r="I47" s="50"/>
       <c r="J47" s="50"/>
-      <c r="K47" s="96"/>
+      <c r="K47" s="92"/>
       <c r="L47" s="87"/>
       <c r="M47" s="51"/>
       <c r="N47" s="51"/>
@@ -5280,7 +5280,7 @@
       <c r="H48" s="50"/>
       <c r="I48" s="50"/>
       <c r="J48" s="50"/>
-      <c r="K48" s="96"/>
+      <c r="K48" s="92"/>
       <c r="L48" s="87"/>
       <c r="M48" s="51"/>
       <c r="N48" s="51"/>
@@ -5296,9 +5296,9 @@
       <c r="H49" s="50"/>
       <c r="I49" s="50"/>
       <c r="J49" s="50"/>
-      <c r="K49" s="96"/>
+      <c r="K49" s="92"/>
       <c r="L49" s="87"/>
-      <c r="M49" s="97" t="s">
+      <c r="M49" s="93" t="s">
         <v>75</v>
       </c>
       <c r="N49" s="51"/>
@@ -5314,9 +5314,9 @@
       <c r="H50" s="50"/>
       <c r="I50" s="50"/>
       <c r="J50" s="50"/>
-      <c r="K50" s="96"/>
+      <c r="K50" s="92"/>
       <c r="L50" s="87"/>
-      <c r="M50" s="97"/>
+      <c r="M50" s="93"/>
       <c r="N50" s="42"/>
       <c r="O50" s="51"/>
       <c r="P50" s="51"/>
@@ -5330,7 +5330,7 @@
       <c r="H51" s="50"/>
       <c r="I51" s="50"/>
       <c r="J51" s="50"/>
-      <c r="K51" s="96" t="s">
+      <c r="K51" s="92" t="s">
         <v>146</v>
       </c>
       <c r="L51" s="87"/>
@@ -5348,7 +5348,7 @@
       <c r="H52" s="50"/>
       <c r="I52" s="50"/>
       <c r="J52" s="50"/>
-      <c r="K52" s="96"/>
+      <c r="K52" s="92"/>
       <c r="L52" s="87"/>
       <c r="M52" s="51"/>
       <c r="N52" s="51"/>
@@ -5364,7 +5364,7 @@
       <c r="H53" s="46"/>
       <c r="I53" s="50"/>
       <c r="J53" s="50"/>
-      <c r="K53" s="96"/>
+      <c r="K53" s="92"/>
       <c r="L53" s="87"/>
       <c r="M53" s="51"/>
       <c r="N53" s="42"/>
@@ -5384,7 +5384,7 @@
       </c>
       <c r="I54" s="50"/>
       <c r="J54" s="50"/>
-      <c r="K54" s="96"/>
+      <c r="K54" s="92"/>
       <c r="L54" s="87"/>
       <c r="M54" s="51"/>
       <c r="N54" s="51"/>
@@ -5400,9 +5400,9 @@
       <c r="H55" s="87"/>
       <c r="I55" s="50"/>
       <c r="J55" s="50"/>
-      <c r="K55" s="96"/>
+      <c r="K55" s="92"/>
       <c r="L55" s="87"/>
-      <c r="M55" s="97" t="s">
+      <c r="M55" s="93" t="s">
         <v>74</v>
       </c>
       <c r="N55" s="51"/>
@@ -5418,9 +5418,9 @@
       <c r="H56" s="48"/>
       <c r="I56" s="50"/>
       <c r="J56" s="50"/>
-      <c r="K56" s="96"/>
+      <c r="K56" s="92"/>
       <c r="L56" s="87"/>
-      <c r="M56" s="97"/>
+      <c r="M56" s="93"/>
       <c r="N56" s="51"/>
       <c r="O56" s="51"/>
       <c r="P56" s="51"/>
@@ -5434,7 +5434,7 @@
       <c r="H57" s="50"/>
       <c r="I57" s="50"/>
       <c r="J57" s="50"/>
-      <c r="K57" s="96" t="s">
+      <c r="K57" s="92" t="s">
         <v>79</v>
       </c>
       <c r="L57" s="87"/>
@@ -5452,7 +5452,7 @@
       <c r="H58" s="50"/>
       <c r="I58" s="50"/>
       <c r="J58" s="50"/>
-      <c r="K58" s="96"/>
+      <c r="K58" s="92"/>
       <c r="L58" s="87"/>
       <c r="M58" s="51"/>
       <c r="N58" s="51"/>
@@ -5468,7 +5468,7 @@
       <c r="H59" s="46"/>
       <c r="I59" s="50"/>
       <c r="J59" s="50"/>
-      <c r="K59" s="96"/>
+      <c r="K59" s="92"/>
       <c r="L59" s="87"/>
       <c r="M59" s="51"/>
       <c r="N59" s="51"/>
@@ -5488,7 +5488,7 @@
       </c>
       <c r="I60" s="50"/>
       <c r="J60" s="50"/>
-      <c r="K60" s="96"/>
+      <c r="K60" s="92"/>
       <c r="L60" s="87"/>
       <c r="M60" s="51"/>
       <c r="N60" s="51"/>
@@ -5504,9 +5504,9 @@
       <c r="H61" s="87"/>
       <c r="I61" s="50"/>
       <c r="J61" s="50"/>
-      <c r="K61" s="96"/>
+      <c r="K61" s="92"/>
       <c r="L61" s="87"/>
-      <c r="M61" s="97" t="s">
+      <c r="M61" s="93" t="s">
         <v>73</v>
       </c>
       <c r="N61" s="51"/>
@@ -5522,9 +5522,9 @@
       <c r="H62" s="48"/>
       <c r="I62" s="50"/>
       <c r="J62" s="50"/>
-      <c r="K62" s="96"/>
+      <c r="K62" s="92"/>
       <c r="L62" s="87"/>
-      <c r="M62" s="97"/>
+      <c r="M62" s="93"/>
       <c r="N62" s="51"/>
       <c r="O62" s="51"/>
       <c r="P62" s="51"/>
@@ -5538,7 +5538,7 @@
       <c r="H63" s="50"/>
       <c r="I63" s="50"/>
       <c r="J63" s="50"/>
-      <c r="K63" s="98" t="s">
+      <c r="K63" s="94" t="s">
         <v>77</v>
       </c>
       <c r="L63" s="87"/>
@@ -5556,7 +5556,7 @@
       <c r="H64" s="50"/>
       <c r="I64" s="50"/>
       <c r="J64" s="50"/>
-      <c r="K64" s="98"/>
+      <c r="K64" s="94"/>
       <c r="L64" s="87"/>
       <c r="M64" s="51"/>
       <c r="N64" s="51"/>
@@ -5572,7 +5572,7 @@
       <c r="H65" s="46"/>
       <c r="I65" s="50"/>
       <c r="J65" s="50"/>
-      <c r="K65" s="98"/>
+      <c r="K65" s="94"/>
       <c r="L65" s="87"/>
       <c r="M65" s="51"/>
       <c r="N65" s="51"/>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="I66" s="50"/>
       <c r="J66" s="50"/>
-      <c r="K66" s="98"/>
+      <c r="K66" s="94"/>
       <c r="L66" s="87"/>
       <c r="M66" s="51"/>
       <c r="N66" s="51"/>
@@ -5598,9 +5598,9 @@
       <c r="H67" s="87"/>
       <c r="I67" s="50"/>
       <c r="J67" s="50"/>
-      <c r="K67" s="98"/>
+      <c r="K67" s="94"/>
       <c r="L67" s="87"/>
-      <c r="M67" s="97" t="s">
+      <c r="M67" s="93" t="s">
         <v>72</v>
       </c>
       <c r="N67" s="51"/>
@@ -5611,9 +5611,9 @@
       <c r="H68" s="48"/>
       <c r="I68" s="50"/>
       <c r="J68" s="50"/>
-      <c r="K68" s="98"/>
+      <c r="K68" s="94"/>
       <c r="L68" s="87"/>
-      <c r="M68" s="97"/>
+      <c r="M68" s="93"/>
       <c r="N68" s="51"/>
       <c r="O68" s="51"/>
     </row>
@@ -5708,19 +5708,19 @@
       </c>
     </row>
     <row r="80" spans="7:16" ht="20">
-      <c r="K80" s="109" t="s">
+      <c r="K80" s="99" t="s">
         <v>166</v>
       </c>
-      <c r="L80" s="108">
+      <c r="L80" s="101">
         <v>10</v>
       </c>
       <c r="M80" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="N80" s="110" t="s">
+      <c r="N80" s="100" t="s">
         <v>165</v>
       </c>
-      <c r="O80" s="108">
+      <c r="O80" s="101">
         <v>0</v>
       </c>
       <c r="P80" s="7" t="s">
@@ -5728,37 +5728,37 @@
       </c>
     </row>
     <row r="81" spans="11:16" ht="20">
-      <c r="K81" s="110"/>
-      <c r="L81" s="108"/>
+      <c r="K81" s="100"/>
+      <c r="L81" s="101"/>
       <c r="M81" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="N81" s="110"/>
-      <c r="O81" s="108"/>
+      <c r="N81" s="100"/>
+      <c r="O81" s="101"/>
       <c r="P81" s="7" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="82" spans="11:16" ht="20">
-      <c r="K82" s="110"/>
-      <c r="L82" s="108"/>
+      <c r="K82" s="100"/>
+      <c r="L82" s="101"/>
       <c r="M82" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="N82" s="110"/>
-      <c r="O82" s="108"/>
+      <c r="N82" s="100"/>
+      <c r="O82" s="101"/>
       <c r="P82" s="7" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="83" spans="11:16" ht="20">
-      <c r="K83" s="110"/>
-      <c r="L83" s="108"/>
+      <c r="K83" s="100"/>
+      <c r="L83" s="101"/>
       <c r="M83" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="N83" s="110"/>
-      <c r="O83" s="108"/>
+      <c r="N83" s="100"/>
+      <c r="O83" s="101"/>
       <c r="P83" s="7" t="s">
         <v>167</v>
       </c>
@@ -5782,7 +5782,7 @@
       <c r="K90" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="L90" s="92" t="s">
+      <c r="L90" s="95" t="s">
         <v>98</v>
       </c>
       <c r="M90" s="31"/>
@@ -5791,44 +5791,44 @@
     </row>
     <row r="91" spans="11:16">
       <c r="K91" s="68"/>
-      <c r="L91" s="93"/>
+      <c r="L91" s="96"/>
       <c r="M91" s="31"/>
       <c r="N91" s="31"/>
       <c r="O91" s="31"/>
     </row>
     <row r="92" spans="11:16">
       <c r="K92" s="68"/>
-      <c r="L92" s="93"/>
+      <c r="L92" s="96"/>
       <c r="M92" s="31"/>
       <c r="N92" s="31"/>
       <c r="O92" s="31"/>
     </row>
     <row r="93" spans="11:16">
       <c r="K93" s="68"/>
-      <c r="L93" s="93"/>
+      <c r="L93" s="96"/>
       <c r="M93" s="31"/>
       <c r="N93" s="31"/>
       <c r="O93" s="31"/>
     </row>
     <row r="94" spans="11:16">
       <c r="K94" s="68"/>
-      <c r="L94" s="93"/>
+      <c r="L94" s="96"/>
     </row>
     <row r="95" spans="11:16">
       <c r="K95" s="68"/>
-      <c r="L95" s="93"/>
+      <c r="L95" s="96"/>
     </row>
     <row r="96" spans="11:16">
       <c r="K96" s="68"/>
-      <c r="L96" s="93"/>
+      <c r="L96" s="96"/>
     </row>
     <row r="97" spans="11:15">
       <c r="K97" s="68"/>
-      <c r="L97" s="94"/>
+      <c r="L97" s="97"/>
     </row>
     <row r="98" spans="11:15">
       <c r="K98" s="68"/>
-      <c r="L98" s="95" t="s">
+      <c r="L98" s="98" t="s">
         <v>100</v>
       </c>
       <c r="M98" s="31"/>
@@ -5837,22 +5837,22 @@
     </row>
     <row r="99" spans="11:15">
       <c r="K99" s="68"/>
-      <c r="L99" s="95"/>
+      <c r="L99" s="98"/>
       <c r="M99" s="31"/>
       <c r="N99" s="31"/>
       <c r="O99" s="31"/>
     </row>
     <row r="100" spans="11:15">
       <c r="K100" s="68"/>
-      <c r="L100" s="95"/>
+      <c r="L100" s="98"/>
     </row>
     <row r="101" spans="11:15">
       <c r="K101" s="68"/>
-      <c r="L101" s="95"/>
+      <c r="L101" s="98"/>
     </row>
     <row r="102" spans="11:15">
       <c r="K102" s="68"/>
-      <c r="L102" s="95" t="s">
+      <c r="L102" s="98" t="s">
         <v>99</v>
       </c>
       <c r="M102" s="31"/>
@@ -5861,18 +5861,18 @@
     </row>
     <row r="103" spans="11:15">
       <c r="K103" s="68"/>
-      <c r="L103" s="95"/>
+      <c r="L103" s="98"/>
       <c r="M103" s="31"/>
       <c r="N103" s="31"/>
       <c r="O103" s="31"/>
     </row>
     <row r="104" spans="11:15">
       <c r="K104" s="68"/>
-      <c r="L104" s="95"/>
+      <c r="L104" s="98"/>
     </row>
     <row r="105" spans="11:15">
       <c r="K105" s="68"/>
-      <c r="L105" s="95"/>
+      <c r="L105" s="98"/>
     </row>
     <row r="106" spans="11:15">
       <c r="L106" s="21"/>
@@ -5884,7 +5884,7 @@
       <c r="K123" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="L123" s="92" t="s">
+      <c r="L123" s="95" t="s">
         <v>103</v>
       </c>
       <c r="M123" s="31"/>
@@ -5893,44 +5893,44 @@
     </row>
     <row r="124" spans="11:15">
       <c r="K124" s="68"/>
-      <c r="L124" s="93"/>
+      <c r="L124" s="96"/>
       <c r="M124" s="31"/>
       <c r="N124" s="31"/>
       <c r="O124" s="31"/>
     </row>
     <row r="125" spans="11:15">
       <c r="K125" s="68"/>
-      <c r="L125" s="93"/>
+      <c r="L125" s="96"/>
       <c r="M125" s="31"/>
       <c r="N125" s="31"/>
       <c r="O125" s="31"/>
     </row>
     <row r="126" spans="11:15">
       <c r="K126" s="68"/>
-      <c r="L126" s="93"/>
+      <c r="L126" s="96"/>
       <c r="M126" s="31"/>
       <c r="N126" s="31"/>
       <c r="O126" s="31"/>
     </row>
     <row r="127" spans="11:15">
       <c r="K127" s="68"/>
-      <c r="L127" s="93"/>
+      <c r="L127" s="96"/>
     </row>
     <row r="128" spans="11:15">
       <c r="K128" s="68"/>
-      <c r="L128" s="93"/>
+      <c r="L128" s="96"/>
     </row>
     <row r="129" spans="3:15">
       <c r="K129" s="68"/>
-      <c r="L129" s="93"/>
+      <c r="L129" s="96"/>
     </row>
     <row r="130" spans="3:15">
       <c r="K130" s="68"/>
-      <c r="L130" s="94"/>
+      <c r="L130" s="97"/>
     </row>
     <row r="131" spans="3:15">
       <c r="K131" s="68"/>
-      <c r="L131" s="95" t="s">
+      <c r="L131" s="98" t="s">
         <v>104</v>
       </c>
       <c r="M131" s="31"/>
@@ -5939,18 +5939,18 @@
     </row>
     <row r="132" spans="3:15">
       <c r="K132" s="68"/>
-      <c r="L132" s="95"/>
+      <c r="L132" s="98"/>
       <c r="M132" s="31"/>
       <c r="N132" s="31"/>
       <c r="O132" s="31"/>
     </row>
     <row r="133" spans="3:15">
       <c r="K133" s="68"/>
-      <c r="L133" s="95"/>
+      <c r="L133" s="98"/>
     </row>
     <row r="134" spans="3:15">
       <c r="K134" s="68"/>
-      <c r="L134" s="95"/>
+      <c r="L134" s="98"/>
     </row>
     <row r="135" spans="3:15">
       <c r="K135" s="32"/>
@@ -6437,15 +6437,6 @@
     <mergeCell ref="AT19:AT22"/>
     <mergeCell ref="AU19:AU22"/>
     <mergeCell ref="AM21:AM24"/>
-    <mergeCell ref="Q9:Q12"/>
-    <mergeCell ref="Q13:Q16"/>
-    <mergeCell ref="Q17:Q20"/>
-    <mergeCell ref="Q21:Q24"/>
-    <mergeCell ref="R9:R12"/>
-    <mergeCell ref="R13:R16"/>
-    <mergeCell ref="R17:R20"/>
-    <mergeCell ref="R21:R24"/>
-    <mergeCell ref="V9:V12"/>
     <mergeCell ref="W9:W12"/>
     <mergeCell ref="V13:V16"/>
     <mergeCell ref="W13:W16"/>
@@ -6460,6 +6451,15 @@
     <mergeCell ref="AP15:AP18"/>
     <mergeCell ref="AP19:AP22"/>
     <mergeCell ref="L39:L44"/>
+    <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="Q13:Q16"/>
+    <mergeCell ref="Q17:Q20"/>
+    <mergeCell ref="Q21:Q24"/>
+    <mergeCell ref="R9:R12"/>
+    <mergeCell ref="R13:R16"/>
+    <mergeCell ref="R17:R20"/>
+    <mergeCell ref="R21:R24"/>
+    <mergeCell ref="V9:V12"/>
     <mergeCell ref="K39:K44"/>
     <mergeCell ref="K45:K50"/>
     <mergeCell ref="L45:L50"/>

</xml_diff>